<commit_message>
add new test backpropagation
</commit_message>
<xml_diff>
--- a/JST_HEBB_BACKPROPAGATION.xlsx
+++ b/JST_HEBB_BACKPROPAGATION.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metode Hebb" sheetId="1" r:id="rId1"/>
     <sheet name="Metode Backpropagation" sheetId="2" r:id="rId2"/>
     <sheet name="Backpropagation Matlab" sheetId="3" r:id="rId3"/>
+    <sheet name="Backpropagation Matlab 2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="67">
   <si>
     <t>Target</t>
   </si>
@@ -1049,13 +1050,22 @@
       </rPr>
       <t/>
     </r>
+  </si>
+  <si>
+    <t>Data Transpose Pengenalan Wajah</t>
+  </si>
+  <si>
+    <t>Data Sample</t>
+  </si>
+  <si>
+    <t>Data Target</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1246,8 +1256,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF4E4E4E"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1296,8 +1320,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1351,11 +1387,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1426,6 +1471,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4947,7 +5000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
@@ -5789,4 +5842,348 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:P18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="40"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="42">
+        <v>0.35</v>
+      </c>
+      <c r="C6" s="42">
+        <v>0.59</v>
+      </c>
+      <c r="D6" s="42">
+        <v>0.19</v>
+      </c>
+      <c r="E6" s="42">
+        <v>0.36</v>
+      </c>
+      <c r="F6" s="42">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G6" s="42">
+        <v>0.4</v>
+      </c>
+      <c r="H6" s="42">
+        <v>0.61</v>
+      </c>
+      <c r="I6" s="42">
+        <v>0.2</v>
+      </c>
+      <c r="J6" s="42">
+        <v>0.38</v>
+      </c>
+      <c r="K6" s="42">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="L6" s="42">
+        <v>0.33</v>
+      </c>
+      <c r="M6" s="42">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="N6" s="42">
+        <v>0.18</v>
+      </c>
+      <c r="O6" s="42">
+        <v>0.38</v>
+      </c>
+      <c r="P6" s="42">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="42">
+        <v>0.47</v>
+      </c>
+      <c r="C7" s="42">
+        <v>0.11</v>
+      </c>
+      <c r="D7" s="42">
+        <v>0.89</v>
+      </c>
+      <c r="E7" s="42">
+        <v>0.9</v>
+      </c>
+      <c r="F7" s="42">
+        <v>0.45</v>
+      </c>
+      <c r="G7" s="42">
+        <v>0.45</v>
+      </c>
+      <c r="H7" s="42">
+        <v>0.11</v>
+      </c>
+      <c r="I7" s="42">
+        <v>0.87</v>
+      </c>
+      <c r="J7" s="42">
+        <v>0.88</v>
+      </c>
+      <c r="K7" s="42">
+        <v>0.46</v>
+      </c>
+      <c r="L7" s="42">
+        <v>0.45</v>
+      </c>
+      <c r="M7" s="42">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N7" s="42">
+        <v>0.87</v>
+      </c>
+      <c r="O7" s="42">
+        <v>0.89</v>
+      </c>
+      <c r="P7" s="42">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="42">
+        <v>0.88</v>
+      </c>
+      <c r="C8" s="42">
+        <v>0.9</v>
+      </c>
+      <c r="D8" s="42">
+        <v>0.54</v>
+      </c>
+      <c r="E8" s="42">
+        <v>0.39</v>
+      </c>
+      <c r="F8" s="42">
+        <v>0.8</v>
+      </c>
+      <c r="G8" s="42">
+        <v>0.8</v>
+      </c>
+      <c r="H8" s="42">
+        <v>0.9</v>
+      </c>
+      <c r="I8" s="42">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J8" s="42">
+        <v>0.35</v>
+      </c>
+      <c r="K8" s="42">
+        <v>0.82</v>
+      </c>
+      <c r="L8" s="42">
+        <v>0.85</v>
+      </c>
+      <c r="M8" s="42">
+        <v>0.9</v>
+      </c>
+      <c r="N8" s="42">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O8" s="42">
+        <v>0.37</v>
+      </c>
+      <c r="P8" s="42">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="42">
+        <v>0.34</v>
+      </c>
+      <c r="C9" s="42">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D9" s="42">
+        <v>0.38</v>
+      </c>
+      <c r="E9" s="42">
+        <v>0.82</v>
+      </c>
+      <c r="F9" s="42">
+        <v>0.91</v>
+      </c>
+      <c r="G9" s="42">
+        <v>0.35</v>
+      </c>
+      <c r="H9" s="42">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I9" s="42">
+        <v>0.41</v>
+      </c>
+      <c r="J9" s="42">
+        <v>0.85</v>
+      </c>
+      <c r="K9" s="42">
+        <v>0.92</v>
+      </c>
+      <c r="L9" s="42">
+        <v>0.37</v>
+      </c>
+      <c r="M9" s="42">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="N9" s="42">
+        <v>0.4</v>
+      </c>
+      <c r="O9" s="42">
+        <v>0.85</v>
+      </c>
+      <c r="P9" s="42">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="11"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="43">
+        <v>1</v>
+      </c>
+      <c r="C12" s="43">
+        <v>2</v>
+      </c>
+      <c r="D12" s="43">
+        <v>3</v>
+      </c>
+      <c r="E12" s="43">
+        <v>4</v>
+      </c>
+      <c r="F12" s="43">
+        <v>5</v>
+      </c>
+      <c r="G12" s="43">
+        <v>1</v>
+      </c>
+      <c r="H12" s="43">
+        <v>2</v>
+      </c>
+      <c r="I12" s="43">
+        <v>3</v>
+      </c>
+      <c r="J12" s="43">
+        <v>4</v>
+      </c>
+      <c r="K12" s="43">
+        <v>5</v>
+      </c>
+      <c r="L12" s="43">
+        <v>1</v>
+      </c>
+      <c r="M12" s="43">
+        <v>2</v>
+      </c>
+      <c r="N12" s="43">
+        <v>3</v>
+      </c>
+      <c r="O12" s="43">
+        <v>4</v>
+      </c>
+      <c r="P12" s="43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="42">
+        <v>0.38</v>
+      </c>
+      <c r="C15" s="42">
+        <v>0.6</v>
+      </c>
+      <c r="D15" s="42">
+        <v>0.19</v>
+      </c>
+      <c r="E15" s="42">
+        <v>0.35</v>
+      </c>
+      <c r="F15" s="42">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="42">
+        <v>0.43</v>
+      </c>
+      <c r="C16" s="42">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D16" s="42">
+        <v>0.88</v>
+      </c>
+      <c r="E16" s="42">
+        <v>0.9</v>
+      </c>
+      <c r="F16" s="42">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="43">
+        <v>0.85</v>
+      </c>
+      <c r="C17" s="43">
+        <v>0.87</v>
+      </c>
+      <c r="D17" s="43">
+        <v>0.6</v>
+      </c>
+      <c r="E17" s="43">
+        <v>0.41</v>
+      </c>
+      <c r="F17" s="43">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="42">
+        <v>0.34</v>
+      </c>
+      <c r="C18" s="42">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D18" s="42">
+        <v>0.4</v>
+      </c>
+      <c r="E18" s="42">
+        <v>0.83</v>
+      </c>
+      <c r="F18" s="42">
+        <v>0.93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>